<commit_message>
not yet contacted list
</commit_message>
<xml_diff>
--- a/accepted.xlsx
+++ b/accepted.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="502">
   <si>
     <t>Full Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Foulen El Fouleni</t>
-  </si>
-  <si>
     <t>Achraf Ben Soltane</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
     <t>Ali karfouh</t>
   </si>
   <si>
+    <t>Amal Albouchi</t>
+  </si>
+  <si>
     <t>AMMAR Mohamed Ayoub</t>
   </si>
   <si>
@@ -70,12 +70,24 @@
     <t>atef haj ahmed</t>
   </si>
   <si>
+    <t>Hamza Laabidi</t>
+  </si>
+  <si>
+    <t>Chraiti Rafed</t>
+  </si>
+  <si>
+    <t>Daoudi Ahmed</t>
+  </si>
+  <si>
     <t>eya el miziaine</t>
   </si>
   <si>
     <t>Besrour Sarra</t>
   </si>
   <si>
+    <t>fedi amine ladhari</t>
+  </si>
+  <si>
     <t>Eya karmous</t>
   </si>
   <si>
@@ -100,6 +112,12 @@
     <t>Hammadi Meriem</t>
   </si>
   <si>
+    <t>hiba annak</t>
+  </si>
+  <si>
+    <t>iyed ben massoud</t>
+  </si>
+  <si>
     <t>jazi amal</t>
   </si>
   <si>
@@ -127,6 +145,9 @@
     <t>Makhlouf Ala Eddine</t>
   </si>
   <si>
+    <t>Malek Belhadj</t>
+  </si>
+  <si>
     <t>Maram Bakini</t>
   </si>
   <si>
@@ -199,6 +220,9 @@
     <t>Salma soula</t>
   </si>
   <si>
+    <t>Oueslati Sawssen</t>
+  </si>
+  <si>
     <t>Oussema ibn fraj</t>
   </si>
   <si>
@@ -226,6 +250,9 @@
     <t>Wassim Malouch</t>
   </si>
   <si>
+    <t>Yacoubi Nour El Houda</t>
+  </si>
+  <si>
     <t>Yasmine labassi</t>
   </si>
   <si>
@@ -235,9 +262,6 @@
     <t>Youssef Maaouia</t>
   </si>
   <si>
-    <t>1234678.0</t>
-  </si>
-  <si>
     <t>20154257.0</t>
   </si>
   <si>
@@ -247,6 +271,9 @@
     <t>21631400.0</t>
   </si>
   <si>
+    <t>92212196.0</t>
+  </si>
+  <si>
     <t>50235431.0</t>
   </si>
   <si>
@@ -256,12 +283,24 @@
     <t>56852634.0</t>
   </si>
   <si>
+    <t>54787432.0</t>
+  </si>
+  <si>
+    <t>22611458.0</t>
+  </si>
+  <si>
+    <t>20038175.0</t>
+  </si>
+  <si>
     <t>53469005.0</t>
   </si>
   <si>
     <t>55456978.0</t>
   </si>
   <si>
+    <t>95128230.0</t>
+  </si>
+  <si>
     <t>29681609.0</t>
   </si>
   <si>
@@ -286,6 +325,12 @@
     <t>93781035.0</t>
   </si>
   <si>
+    <t>26202951.0</t>
+  </si>
+  <si>
+    <t>52989546.0</t>
+  </si>
+  <si>
     <t>58175046.0</t>
   </si>
   <si>
@@ -313,6 +358,9 @@
     <t>23911303.0</t>
   </si>
   <si>
+    <t>25667661.0</t>
+  </si>
+  <si>
     <t>20518640.0</t>
   </si>
   <si>
@@ -385,6 +433,9 @@
     <t>51560057.0</t>
   </si>
   <si>
+    <t>29606373.0</t>
+  </si>
+  <si>
     <t>28494765.0</t>
   </si>
   <si>
@@ -412,6 +463,9 @@
     <t>50180757.0</t>
   </si>
   <si>
+    <t>95642327.0</t>
+  </si>
+  <si>
     <t>27790136.0</t>
   </si>
   <si>
@@ -421,9 +475,6 @@
     <t>29763273.0</t>
   </si>
   <si>
-    <t>foulenEl.fouleni@email.com</t>
-  </si>
-  <si>
     <t>achrafb.s2015@gmail.com</t>
   </si>
   <si>
@@ -433,6 +484,9 @@
     <t>zyasuo24@gmail.com</t>
   </si>
   <si>
+    <t>amalalbouchi@gmail.com</t>
+  </si>
+  <si>
     <t>ayoub.ammr@gmail.com</t>
   </si>
   <si>
@@ -442,12 +496,24 @@
     <t>atefhajahmed90@gmail.com</t>
   </si>
   <si>
+    <t>hamzalaabidi71@gmail.com</t>
+  </si>
+  <si>
+    <t>rafed.chraiti99@gmail.com</t>
+  </si>
+  <si>
+    <t>Ahmeddaoudi386@gmail.com</t>
+  </si>
+  <si>
     <t>eyaelmiziaine083@outlook.fr</t>
   </si>
   <si>
     <t>Besroursarra2016@gmail.com</t>
   </si>
   <si>
+    <t>fe-di2012@live.fr</t>
+  </si>
+  <si>
     <t>Eyakarmous779@gmail.com</t>
   </si>
   <si>
@@ -472,6 +538,12 @@
     <t>hammadimeriem754@gmail.com</t>
   </si>
   <si>
+    <t>hibaannak10@gmail.com</t>
+  </si>
+  <si>
+    <t>aymenbenmassoud1@gmail.com</t>
+  </si>
+  <si>
     <t>amzijz002@gmail com</t>
   </si>
   <si>
@@ -499,6 +571,9 @@
     <t>Makhloufalaeddine@gmail.com</t>
   </si>
   <si>
+    <t>Hbhmalek@gmail.com</t>
+  </si>
+  <si>
     <t>marambakini17@gmail.com</t>
   </si>
   <si>
@@ -571,6 +646,9 @@
     <t>Salmasoula20@gmail.com</t>
   </si>
   <si>
+    <t>oueslatisawssen58@gmail.com</t>
+  </si>
+  <si>
     <t>ofradj@gmail.com</t>
   </si>
   <si>
@@ -598,6 +676,9 @@
     <t>Wassimmalouch2001@gmail.com</t>
   </si>
   <si>
+    <t>Nourelhouday2002@gmail.com</t>
+  </si>
+  <si>
     <t>Yasminelabassi08@gmail.com</t>
   </si>
   <si>
@@ -607,9 +688,6 @@
     <t>youssef.maaouia@etudiant-isi.utm.tn</t>
   </si>
   <si>
-    <t>https://facebook.com/foulen.fouleni or Foulen Fouleni</t>
-  </si>
-  <si>
     <t>https://www.facebook.com/achrefoo/</t>
   </si>
   <si>
@@ -619,18 +697,33 @@
     <t>https://m.facebook.com/100003872844516/</t>
   </si>
   <si>
+    <t>https://facebook.com/amal.albouchi</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/ReznoveM/</t>
   </si>
   <si>
     <t>https://www.facebook.com/profile.php?id=100041198479753</t>
   </si>
   <si>
+    <t>https://www.facebook.com/hamza.laabidi.545/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100015393072353</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100008702584258</t>
+  </si>
+  <si>
     <t>https://m.facebook.com/?_rdr</t>
   </si>
   <si>
     <t>https://www.facebook.com/sarra.besrour.5</t>
   </si>
   <si>
+    <t>https://www.facebook.com/ladhari.fedi</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/eya.karmouss</t>
   </si>
   <si>
@@ -655,6 +748,9 @@
     <t>Hammadi meryem</t>
   </si>
   <si>
+    <t>IYED BEN MASSOUD</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/jazi.amal.165/</t>
   </si>
   <si>
@@ -682,6 +778,9 @@
     <t>https://m.facebook.com/100000062370346/</t>
   </si>
   <si>
+    <t>https://www.facebook.com/profile.php?id=100008638750840</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/maram.bakini   https://www.instagram.com/maram_bakini/</t>
   </si>
   <si>
@@ -775,27 +874,9 @@
     <t>https://m.facebook.com/maaouia.youssef</t>
   </si>
   <si>
-    <t>2021-09-30 13:35:00</t>
-  </si>
-  <si>
-    <t>7/10/2021 13h</t>
-  </si>
-  <si>
-    <t>07/10/2021 13h20</t>
-  </si>
-  <si>
-    <t>07/10/2021 11h11</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
-    <t>le 6 octobre 15h</t>
-  </si>
-  <si>
-    <t>A205 ou El Local</t>
-  </si>
-  <si>
     <t>unspec</t>
   </si>
   <si>
@@ -805,15 +886,15 @@
     <t>locale</t>
   </si>
   <si>
+    <t>local</t>
+  </si>
+  <si>
     <t xml:space="preserve">unspecified </t>
   </si>
   <si>
     <t>balcon</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
     <t xml:space="preserve">local </t>
   </si>
   <si>
@@ -823,9 +904,6 @@
     <t>A207</t>
   </si>
   <si>
-    <t>Ilyes Helal</t>
-  </si>
-  <si>
     <t>mohamed fares</t>
   </si>
   <si>
@@ -838,12 +916,18 @@
     <t>wiem saadi</t>
   </si>
   <si>
+    <t>Amine Ben Mansour</t>
+  </si>
+  <si>
     <t>yessine</t>
   </si>
   <si>
     <t>HADIL</t>
   </si>
   <si>
+    <t>fatma</t>
+  </si>
+  <si>
     <t>hedi</t>
   </si>
   <si>
@@ -862,6 +946,9 @@
     <t>maram</t>
   </si>
   <si>
+    <t>hadil</t>
+  </si>
+  <si>
     <t>ilyes</t>
   </si>
   <si>
@@ -880,6 +967,9 @@
     <t>fatma bZ</t>
   </si>
   <si>
+    <t>saif</t>
+  </si>
+  <si>
     <t>saif dhifi/khlil</t>
   </si>
   <si>
@@ -907,15 +997,15 @@
     <t>Med ilyes Helal</t>
   </si>
   <si>
-    <t>Amine Ben Mansour</t>
-  </si>
-  <si>
     <t>0.0</t>
   </si>
   <si>
     <t>fatma bouzouita</t>
   </si>
   <si>
+    <t xml:space="preserve">malek bokri </t>
+  </si>
+  <si>
     <t>moatar sellami</t>
   </si>
   <si>
@@ -940,21 +1030,12 @@
     <t>moktar sellami</t>
   </si>
   <si>
-    <t>saif</t>
-  </si>
-  <si>
-    <t>Yes = Accepted No + Red Color Column = Denied</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>HLP HR</t>
-  </si>
-  <si>
     <t>PS</t>
   </si>
   <si>
@@ -964,12 +1045,18 @@
     <t>robotics</t>
   </si>
   <si>
+    <t>ps</t>
+  </si>
+  <si>
     <t xml:space="preserve">PS department </t>
   </si>
   <si>
     <t>PS department</t>
   </si>
   <si>
+    <t>HLP</t>
+  </si>
+  <si>
     <t>hlp/ps</t>
   </si>
   <si>
@@ -991,9 +1078,6 @@
     <t>ps/ hlp</t>
   </si>
   <si>
-    <t>ps</t>
-  </si>
-  <si>
     <t>HR/ROBOTIC</t>
   </si>
   <si>
@@ -1015,6 +1099,9 @@
     <t>HLP/PS</t>
   </si>
   <si>
+    <t>Ps/HLP</t>
+  </si>
+  <si>
     <t>PS/HR</t>
   </si>
   <si>
@@ -1081,15 +1168,15 @@
     <t>ps/HR</t>
   </si>
   <si>
-    <t>2000-02-19 00:00:00</t>
-  </si>
-  <si>
     <t>1999-07-08 00:00:00</t>
   </si>
   <si>
     <t>2003-01-29 00:00:00</t>
   </si>
   <si>
+    <t>1998-03-09 00:00:00</t>
+  </si>
+  <si>
     <t>1999-09-21 00:00:00</t>
   </si>
   <si>
@@ -1099,12 +1186,18 @@
     <t>11\09\2002</t>
   </si>
   <si>
+    <t>1999-08-13 00:00:00</t>
+  </si>
+  <si>
     <t>2021-06-05 00:00:00</t>
   </si>
   <si>
     <t>2021-07-31 00:00:00</t>
   </si>
   <si>
+    <t>2021-10-18 00:00:00</t>
+  </si>
+  <si>
     <t>2021-07-28 00:00:00</t>
   </si>
   <si>
@@ -1129,6 +1222,9 @@
     <t>2021-04-29 00:00:00</t>
   </si>
   <si>
+    <t>2021-10-08 00:00:00</t>
+  </si>
+  <si>
     <t>2002-12-16 00:00:00</t>
   </si>
   <si>
@@ -1156,6 +1252,9 @@
     <t>2001-06-11 00:00:00</t>
   </si>
   <si>
+    <t>15 April 2002</t>
+  </si>
+  <si>
     <t>2002-05-17 00:00:00</t>
   </si>
   <si>
@@ -1225,6 +1324,9 @@
     <t>2001-04-06 00:00:00</t>
   </si>
   <si>
+    <t>1999-02-09 00:00:00</t>
+  </si>
+  <si>
     <t>28\07\1999</t>
   </si>
   <si>
@@ -1249,6 +1351,9 @@
     <t>2002-02-11 00:00:00</t>
   </si>
   <si>
+    <t>2002-12-29 00:00:00</t>
+  </si>
+  <si>
     <t>17\09\2002</t>
   </si>
   <si>
@@ -1258,13 +1363,13 @@
     <t>2001-08-05 00:00:00</t>
   </si>
   <si>
-    <t>In other clubs / other informations</t>
-  </si>
-  <si>
     <t>jawou fesfes ; i7eb i5dem aalkher aal public speaking mté3ou wl team collaboration</t>
   </si>
   <si>
-    <t>likes to work in groups/flexible/aandou chaine youtube, maghroum bel montage wel editing</t>
+    <t>likes to work in groups/flexible/aandou chaine youtube, maghroum bel montage wel editing, yasla7 barcha lel marketing</t>
+  </si>
+  <si>
+    <t>interested in competitive programming/doesnt give up easily/motivated w jawha behi aalekher</t>
   </si>
   <si>
     <t>mern stack , nrah future formateur / oumour mindset yecer tayara / éma khsara mch HLP dept :(</t>
@@ -1276,12 +1381,24 @@
     <t>aandou exp fi robotics behya, kal yheb ydkhol robotics and HR ama mahouch taaa HR khater doesnt know how to deal with issues, doesnt deal with disagreements.</t>
   </si>
   <si>
+    <t>no past experiences/interested in PS/no top tech skills (par rapport l wehed 1ing c'est dommage) ama cv mouch khayeb</t>
+  </si>
+  <si>
+    <t>lezmou n pushiweh akther éma jawou behy ; ifhem basic web dev html css php ..</t>
+  </si>
+  <si>
+    <t>GG aalkher, DevOps, gitlab, github ifhem dev w yecer cool</t>
+  </si>
+  <si>
     <t>good language skills / travailleuse/elle a la volanté</t>
   </si>
   <si>
     <t>AMBITIOUS/EASY GOING/timide/tra rou7ha leader/anglais+allment</t>
   </si>
   <si>
+    <t>il a une grande experience dans les club et il prend beaucoup de postes/il a assité a plein des event/active/yet3allem fissa3 w y7eb y3allem/y2ajjel l7ajet /y7eb organisation/mcherek fi google w securinet</t>
+  </si>
+  <si>
     <t>langue :very good/montage vedeo +</t>
   </si>
   <si>
@@ -1295,6 +1412,9 @@
   </si>
   <si>
     <t xml:space="preserve">creative /ponctuelle -metsarra3/lazy/skills:montage vedeo/Developpementweb/java/c/cherek fi barcha clubet w ken team </t>
+  </si>
+  <si>
+    <t>vis presedent fi leo club/autre club non lucratif/good in organisation /il a un projet qui veut realiser/craetive /communicant/tres serieux et nerveux un peu/techniquement:c/c++/un peu de java /ychouf rou7ou leader</t>
   </si>
   <si>
     <t>Strength : active, self confidance, sociable
@@ -1320,6 +1440,9 @@
     <t xml:space="preserve">HTML basics  /  PHP </t>
   </si>
   <si>
+    <t>previous bureau experience/ basic PS experince/ motivated</t>
+  </si>
+  <si>
     <t xml:space="preserve">zero knowledge in FOSS but impressed with the culture
 </t>
   </si>
@@ -1373,6 +1496,9 @@
   </si>
   <si>
     <t xml:space="preserve">advanced in HTML CSS JAVA JAVASCRIPT SQL ////// vie associative leo </t>
+  </si>
+  <si>
+    <t>motivated aalkher w théb tekhdem fi dep ps w tal3ab m3a team fi competitions</t>
   </si>
   <si>
     <t>Strength : fast lerning
@@ -1391,6 +1517,9 @@
   <si>
     <t>Html css java sql c hlp w ps
 Maynajamch yji team leader,</t>
+  </si>
+  <si>
+    <t>m3a club ekher + 3andha chwaya bokhl ama ki tebda tekhdm thot fi 9albha + fehma principe taa el free software + theb tkoun active</t>
   </si>
   <si>
     <t>introvert, no exp in marketing and robotics, khawefa, motivated bech tekhdem , hard worker</t>
@@ -1770,7 +1899,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1819,34 +1948,34 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>197</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>253</v>
+        <v>286</v>
       </c>
       <c r="G2" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
       <c r="H2" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="I2" t="s">
-        <v>309</v>
+        <v>338</v>
       </c>
       <c r="J2" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="K2" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="L2" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1857,34 +1986,34 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>198</v>
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>225</v>
       </c>
       <c r="F3" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="G3" t="s">
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="H3" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="I3" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J3" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="K3" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="L3" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1895,34 +2024,28 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" t="s">
-        <v>199</v>
+        <v>155</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="F4" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="G4" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="H4" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="I4" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J4" t="s">
-        <v>314</v>
-      </c>
-      <c r="K4" t="s">
-        <v>357</v>
-      </c>
-      <c r="L4" t="s">
-        <v>416</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1933,28 +2056,34 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>200</v>
+        <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="G5" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="H5" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="I5" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J5" t="s">
-        <v>315</v>
+        <v>343</v>
+      </c>
+      <c r="K5" t="s">
+        <v>386</v>
+      </c>
+      <c r="L5" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1965,34 +2094,34 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
       <c r="F6" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G6" t="s">
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="H6" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="I6" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J6" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="K6" t="s">
-        <v>358</v>
+        <v>387</v>
       </c>
       <c r="L6" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2003,34 +2132,34 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>202</v>
+        <v>229</v>
       </c>
       <c r="F7" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G7" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="H7" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="I7" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J7" t="s">
-        <v>317</v>
+        <v>345</v>
       </c>
       <c r="K7" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="L7" t="s">
-        <v>418</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2041,34 +2170,34 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G8" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H8" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="I8" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J8" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="K8" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
       <c r="L8" t="s">
-        <v>419</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2079,34 +2208,34 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="F9" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G9" t="s">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="H9" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="I9" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J9" t="s">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="K9" t="s">
-        <v>361</v>
+        <v>390</v>
       </c>
       <c r="L9" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2117,31 +2246,31 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>204</v>
+        <v>231</v>
       </c>
       <c r="F10" t="s">
-        <v>257</v>
+        <v>286</v>
+      </c>
+      <c r="G10" t="s">
+        <v>287</v>
       </c>
       <c r="H10" t="s">
-        <v>275</v>
+        <v>300</v>
       </c>
       <c r="I10" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="J10" t="s">
-        <v>319</v>
-      </c>
-      <c r="K10" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="L10" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2152,34 +2281,31 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="F11" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G11" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="H11" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="I11" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J11" t="s">
-        <v>320</v>
-      </c>
-      <c r="K11" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="L11" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2190,34 +2316,34 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="F12" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G12" t="s">
-        <v>257</v>
+        <v>292</v>
       </c>
       <c r="H12" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="I12" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J12" t="s">
-        <v>321</v>
+        <v>347</v>
       </c>
       <c r="K12" t="s">
-        <v>364</v>
+        <v>391</v>
       </c>
       <c r="L12" t="s">
-        <v>423</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2228,31 +2354,31 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
-      </c>
-      <c r="G13" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="H13" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="I13" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="J13" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="K13" t="s">
-        <v>365</v>
+        <v>392</v>
+      </c>
+      <c r="L13" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2263,34 +2389,34 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="F14" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G14" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H14" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="I14" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J14" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="K14" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="L14" t="s">
-        <v>424</v>
+        <v>460</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2301,31 +2427,34 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="F15" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G15" t="s">
-        <v>261</v>
+        <v>289</v>
+      </c>
+      <c r="H15" t="s">
+        <v>304</v>
       </c>
       <c r="I15" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J15" t="s">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="K15" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="L15" t="s">
-        <v>425</v>
+        <v>461</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2336,34 +2465,34 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G16" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="H16" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="I16" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J16" t="s">
-        <v>324</v>
+        <v>350</v>
       </c>
       <c r="K16" t="s">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="L16" t="s">
-        <v>426</v>
+        <v>462</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2374,31 +2503,31 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
       <c r="F17" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G17" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H17" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="I17" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J17" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="K17" t="s">
-        <v>369</v>
+        <v>396</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2409,31 +2538,34 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" t="s">
-        <v>212</v>
+        <v>169</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G18" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="H18" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="I18" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J18" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="K18" t="s">
-        <v>370</v>
+        <v>397</v>
+      </c>
+      <c r="L18" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2444,34 +2576,31 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="F19" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G19" t="s">
-        <v>261</v>
-      </c>
-      <c r="H19" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="I19" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J19" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="K19" t="s">
-        <v>371</v>
+        <v>398</v>
       </c>
       <c r="L19" t="s">
-        <v>427</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2482,34 +2611,34 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="F20" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G20" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="H20" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="I20" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J20" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
       <c r="K20" t="s">
-        <v>372</v>
+        <v>399</v>
       </c>
       <c r="L20" t="s">
-        <v>428</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2520,31 +2649,31 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G21" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="H21" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="I21" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J21" t="s">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="K21" t="s">
-        <v>373</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2555,34 +2684,31 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>216</v>
+        <v>173</v>
+      </c>
+      <c r="E22" t="s">
+        <v>243</v>
       </c>
       <c r="F22" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G22" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="H22" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="I22" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J22" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="K22" t="s">
-        <v>374</v>
-      </c>
-      <c r="L22" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2593,34 +2719,22 @@
         <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G23" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="H23" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="I23" t="s">
-        <v>310</v>
-      </c>
-      <c r="J23" t="s">
-        <v>329</v>
-      </c>
-      <c r="K23" t="s">
-        <v>375</v>
-      </c>
-      <c r="L23" t="s">
-        <v>430</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2631,31 +2745,34 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="F24" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G24" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H24" t="s">
-        <v>282</v>
+        <v>310</v>
       </c>
       <c r="I24" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J24" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="K24" t="s">
-        <v>376</v>
+        <v>402</v>
+      </c>
+      <c r="L24" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2666,28 +2783,34 @@
         <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="F25" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G25" t="s">
-        <v>265</v>
+        <v>288</v>
+      </c>
+      <c r="H25" t="s">
+        <v>311</v>
       </c>
       <c r="I25" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J25" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="K25" t="s">
-        <v>377</v>
+        <v>403</v>
+      </c>
+      <c r="L25" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2698,34 +2821,34 @@
         <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="F26" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G26" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="H26" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="I26" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J26" t="s">
-        <v>327</v>
+        <v>354</v>
       </c>
       <c r="K26" t="s">
-        <v>378</v>
+        <v>404</v>
       </c>
       <c r="L26" t="s">
-        <v>431</v>
+        <v>468</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2736,34 +2859,31 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="F27" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G27" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H27" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="I27" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J27" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="K27" t="s">
-        <v>379</v>
-      </c>
-      <c r="L27" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2774,34 +2894,34 @@
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="F28" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G28" t="s">
-        <v>262</v>
+        <v>288</v>
       </c>
       <c r="H28" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="I28" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J28" t="s">
-        <v>332</v>
+        <v>356</v>
       </c>
       <c r="K28" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="L28" t="s">
-        <v>433</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2812,34 +2932,34 @@
         <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="F29" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G29" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="H29" t="s">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="I29" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J29" t="s">
-        <v>333</v>
+        <v>357</v>
       </c>
       <c r="K29" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="L29" t="s">
-        <v>434</v>
+        <v>470</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2850,31 +2970,31 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>181</v>
+      </c>
+      <c r="E30" t="s">
+        <v>250</v>
       </c>
       <c r="F30" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G30" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="H30" t="s">
-        <v>271</v>
+        <v>311</v>
       </c>
       <c r="I30" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J30" t="s">
-        <v>334</v>
+        <v>358</v>
       </c>
       <c r="K30" t="s">
-        <v>382</v>
-      </c>
-      <c r="L30" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2885,31 +3005,28 @@
         <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>182</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F31" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G31" t="s">
-        <v>265</v>
-      </c>
-      <c r="H31" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="I31" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="J31" t="s">
-        <v>313</v>
+        <v>359</v>
       </c>
       <c r="K31" t="s">
-        <v>383</v>
-      </c>
-      <c r="L31" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2920,34 +3037,34 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D32" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="F32" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G32" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="H32" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="I32" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="J32" t="s">
-        <v>313</v>
+        <v>355</v>
       </c>
       <c r="K32" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="L32" t="s">
-        <v>437</v>
+        <v>471</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2958,34 +3075,34 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="F33" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G33" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H33" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
       <c r="I33" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J33" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="K33" t="s">
-        <v>385</v>
+        <v>411</v>
       </c>
       <c r="L33" t="s">
-        <v>438</v>
+        <v>472</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -2996,34 +3113,34 @@
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="F34" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G34" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H34" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="I34" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J34" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="K34" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="L34" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -3034,34 +3151,34 @@
         <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
-      </c>
-      <c r="E35" t="s">
-        <v>227</v>
+        <v>186</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="F35" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G35" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
       <c r="H35" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="I35" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J35" t="s">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="K35" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="L35" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -3072,34 +3189,34 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G36" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="H36" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="I36" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J36" t="s">
-        <v>337</v>
+        <v>362</v>
       </c>
       <c r="K36" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="L36" t="s">
-        <v>441</v>
+        <v>475</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -3110,34 +3227,31 @@
         <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>229</v>
+        <v>188</v>
       </c>
       <c r="F37" t="s">
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="G37" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H37" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="I37" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="J37" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
       <c r="K37" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="L37" t="s">
-        <v>442</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -3148,34 +3262,31 @@
         <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="D38" t="s">
-        <v>171</v>
-      </c>
-      <c r="E38" t="s">
-        <v>230</v>
+        <v>189</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G38" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H38" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="I38" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="J38" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K38" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="L38" t="s">
-        <v>443</v>
+        <v>477</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -3186,31 +3297,34 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D39" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="F39" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G39" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="H39" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="I39" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="J39" t="s">
         <v>340</v>
       </c>
       <c r="K39" t="s">
-        <v>391</v>
+        <v>417</v>
+      </c>
+      <c r="L39" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -3221,31 +3335,34 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="F40" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G40" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="H40" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="I40" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="J40" t="s">
-        <v>313</v>
+        <v>364</v>
+      </c>
+      <c r="K40" t="s">
+        <v>418</v>
       </c>
       <c r="L40" t="s">
-        <v>444</v>
+        <v>479</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -3256,34 +3373,34 @@
         <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="F41" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G41" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H41" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="I41" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K41" t="s">
-        <v>392</v>
+        <v>419</v>
       </c>
       <c r="L41" t="s">
-        <v>445</v>
+        <v>480</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -3294,34 +3411,34 @@
         <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>234</v>
+        <v>193</v>
+      </c>
+      <c r="E42" t="s">
+        <v>260</v>
       </c>
       <c r="F42" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G42" t="s">
-        <v>265</v>
+        <v>293</v>
       </c>
       <c r="H42" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="I42" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J42" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="K42" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="L42" t="s">
-        <v>446</v>
+        <v>481</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -3332,34 +3449,34 @@
         <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D43" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F43" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G43" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H43" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="I43" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J43" t="s">
-        <v>343</v>
+        <v>366</v>
       </c>
       <c r="K43" t="s">
-        <v>394</v>
+        <v>421</v>
       </c>
       <c r="L43" t="s">
-        <v>447</v>
+        <v>482</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -3370,31 +3487,34 @@
         <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>177</v>
+        <v>195</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F44" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G44" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H44" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="I44" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="J44" t="s">
-        <v>315</v>
+        <v>367</v>
       </c>
       <c r="K44" t="s">
-        <v>395</v>
+        <v>422</v>
       </c>
       <c r="L44" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -3405,28 +3525,34 @@
         <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>178</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>236</v>
+        <v>196</v>
+      </c>
+      <c r="E45" t="s">
+        <v>263</v>
       </c>
       <c r="F45" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G45" t="s">
-        <v>265</v>
+        <v>290</v>
+      </c>
+      <c r="H45" t="s">
+        <v>323</v>
       </c>
       <c r="I45" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J45" t="s">
-        <v>344</v>
+        <v>368</v>
       </c>
       <c r="K45" t="s">
-        <v>396</v>
+        <v>423</v>
+      </c>
+      <c r="L45" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3437,34 +3563,31 @@
         <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="F46" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G46" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H46" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="I46" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J46" t="s">
-        <v>345</v>
+        <v>369</v>
       </c>
       <c r="K46" t="s">
-        <v>397</v>
-      </c>
-      <c r="L46" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3475,31 +3598,31 @@
         <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="F47" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G47" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="H47" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I47" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="J47" t="s">
-        <v>325</v>
-      </c>
-      <c r="K47" t="s">
-        <v>398</v>
+        <v>340</v>
+      </c>
+      <c r="L47" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3510,28 +3633,34 @@
         <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>181</v>
+        <v>199</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="F48" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G48" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H48" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
       <c r="I48" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J48" t="s">
-        <v>325</v>
+        <v>370</v>
       </c>
       <c r="K48" t="s">
-        <v>399</v>
+        <v>425</v>
+      </c>
+      <c r="L48" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3542,31 +3671,34 @@
         <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D49" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="F49" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G49" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H49" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="I49" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J49" t="s">
-        <v>325</v>
+        <v>371</v>
       </c>
       <c r="K49" t="s">
-        <v>400</v>
+        <v>426</v>
+      </c>
+      <c r="L49" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3577,31 +3709,34 @@
         <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="F50" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G50" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H50" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="I50" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J50" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
       <c r="K50" t="s">
-        <v>401</v>
+        <v>427</v>
+      </c>
+      <c r="L50" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3612,34 +3747,31 @@
         <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>184</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="F51" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G51" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H51" t="s">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c r="I51" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J51" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="K51" t="s">
-        <v>402</v>
+        <v>428</v>
       </c>
       <c r="L51" t="s">
-        <v>450</v>
+        <v>489</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3650,31 +3782,28 @@
         <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="F52" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G52" t="s">
-        <v>265</v>
-      </c>
-      <c r="H52" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="I52" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J52" t="s">
-        <v>315</v>
+        <v>373</v>
       </c>
       <c r="K52" t="s">
-        <v>403</v>
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3685,34 +3814,34 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="F53" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G53" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H53" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="I53" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J53" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="K53" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="L53" t="s">
-        <v>451</v>
+        <v>490</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3723,31 +3852,31 @@
         <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="F54" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G54" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H54" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="I54" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J54" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="K54" t="s">
-        <v>405</v>
+        <v>431</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3758,34 +3887,28 @@
         <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
-        <v>188</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="F55" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G55" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H55" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="I55" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J55" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="K55" t="s">
-        <v>406</v>
-      </c>
-      <c r="L55" t="s">
-        <v>452</v>
+        <v>432</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3796,31 +3919,31 @@
         <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s">
-        <v>189</v>
-      </c>
-      <c r="E56" t="s">
-        <v>65</v>
+        <v>207</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="F56" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G56" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="H56" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
       <c r="I56" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J56" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="K56" t="s">
-        <v>407</v>
+        <v>433</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3831,34 +3954,31 @@
         <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="F57" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G57" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="H57" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="I57" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J57" t="s">
-        <v>348</v>
+        <v>375</v>
       </c>
       <c r="K57" t="s">
-        <v>408</v>
-      </c>
-      <c r="L57" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3869,31 +3989,34 @@
         <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="F58" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G58" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H58" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
       <c r="I58" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J58" t="s">
-        <v>342</v>
+        <v>376</v>
       </c>
       <c r="K58" t="s">
-        <v>386</v>
+        <v>435</v>
+      </c>
+      <c r="L58" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3904,34 +4027,31 @@
         <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D59" t="s">
-        <v>192</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="F59" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G59" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H59" t="s">
-        <v>305</v>
+        <v>329</v>
       </c>
       <c r="I59" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J59" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="K59" t="s">
-        <v>409</v>
+        <v>436</v>
       </c>
       <c r="L59" t="s">
-        <v>454</v>
+        <v>492</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3942,34 +4062,31 @@
         <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="F60" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G60" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="H60" t="s">
-        <v>306</v>
+        <v>330</v>
       </c>
       <c r="I60" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J60" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="K60" t="s">
-        <v>410</v>
-      </c>
-      <c r="L60" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -3980,34 +4097,34 @@
         <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>250</v>
+        <v>276</v>
       </c>
       <c r="F61" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G61" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H61" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="I61" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J61" t="s">
-        <v>352</v>
+        <v>377</v>
       </c>
       <c r="K61" t="s">
-        <v>411</v>
+        <v>438</v>
       </c>
       <c r="L61" t="s">
-        <v>456</v>
+        <v>493</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -4018,34 +4135,31 @@
         <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D62" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="F62" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G62" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H62" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="I62" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J62" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="K62" t="s">
-        <v>412</v>
-      </c>
-      <c r="L62" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -4056,40 +4170,373 @@
         <v>72</v>
       </c>
       <c r="C63" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
       <c r="F63" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="G63" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="H63" t="s">
-        <v>308</v>
+        <v>332</v>
       </c>
       <c r="I63" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="J63" t="s">
-        <v>354</v>
+        <v>378</v>
       </c>
       <c r="K63" t="s">
-        <v>413</v>
+        <v>440</v>
       </c>
       <c r="L63" t="s">
-        <v>458</v>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" t="s">
+        <v>144</v>
+      </c>
+      <c r="D64" t="s">
+        <v>215</v>
+      </c>
+      <c r="E64" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" t="s">
+        <v>286</v>
+      </c>
+      <c r="G64" t="s">
+        <v>288</v>
+      </c>
+      <c r="H64" t="s">
+        <v>333</v>
+      </c>
+      <c r="I64" t="s">
+        <v>338</v>
+      </c>
+      <c r="J64" t="s">
+        <v>379</v>
+      </c>
+      <c r="K64" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" t="s">
+        <v>216</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F65" t="s">
+        <v>286</v>
+      </c>
+      <c r="G65" t="s">
+        <v>294</v>
+      </c>
+      <c r="H65" t="s">
+        <v>334</v>
+      </c>
+      <c r="I65" t="s">
+        <v>338</v>
+      </c>
+      <c r="J65" t="s">
+        <v>377</v>
+      </c>
+      <c r="K65" t="s">
+        <v>442</v>
+      </c>
+      <c r="L65" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" t="s">
+        <v>217</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F66" t="s">
+        <v>286</v>
+      </c>
+      <c r="G66" t="s">
+        <v>290</v>
+      </c>
+      <c r="H66" t="s">
+        <v>323</v>
+      </c>
+      <c r="I66" t="s">
+        <v>338</v>
+      </c>
+      <c r="J66" t="s">
+        <v>371</v>
+      </c>
+      <c r="K66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" t="s">
+        <v>218</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F67" t="s">
+        <v>286</v>
+      </c>
+      <c r="G67" t="s">
+        <v>290</v>
+      </c>
+      <c r="H67" t="s">
+        <v>335</v>
+      </c>
+      <c r="I67" t="s">
+        <v>338</v>
+      </c>
+      <c r="J67" t="s">
+        <v>380</v>
+      </c>
+      <c r="K67" t="s">
+        <v>443</v>
+      </c>
+      <c r="L67" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F68" t="s">
+        <v>286</v>
+      </c>
+      <c r="G68" t="s">
+        <v>295</v>
+      </c>
+      <c r="H68" t="s">
+        <v>336</v>
+      </c>
+      <c r="I68" t="s">
+        <v>338</v>
+      </c>
+      <c r="J68" t="s">
+        <v>377</v>
+      </c>
+      <c r="K68" t="s">
+        <v>444</v>
+      </c>
+      <c r="L68" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" t="s">
+        <v>220</v>
+      </c>
+      <c r="F69" t="s">
+        <v>286</v>
+      </c>
+      <c r="G69" t="s">
+        <v>290</v>
+      </c>
+      <c r="H69" t="s">
+        <v>322</v>
+      </c>
+      <c r="I69" t="s">
+        <v>338</v>
+      </c>
+      <c r="J69" t="s">
+        <v>352</v>
+      </c>
+      <c r="K69" t="s">
+        <v>445</v>
+      </c>
+      <c r="L69" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70" t="s">
+        <v>221</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F70" t="s">
+        <v>286</v>
+      </c>
+      <c r="G70" t="s">
+        <v>290</v>
+      </c>
+      <c r="H70" t="s">
+        <v>337</v>
+      </c>
+      <c r="I70" t="s">
+        <v>338</v>
+      </c>
+      <c r="J70" t="s">
+        <v>381</v>
+      </c>
+      <c r="K70" t="s">
+        <v>446</v>
+      </c>
+      <c r="L70" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>151</v>
+      </c>
+      <c r="D71" t="s">
+        <v>222</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F71" t="s">
+        <v>286</v>
+      </c>
+      <c r="G71" t="s">
+        <v>290</v>
+      </c>
+      <c r="H71" t="s">
+        <v>323</v>
+      </c>
+      <c r="I71" t="s">
+        <v>338</v>
+      </c>
+      <c r="J71" t="s">
+        <v>382</v>
+      </c>
+      <c r="K71" t="s">
+        <v>447</v>
+      </c>
+      <c r="L71" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F72" t="s">
+        <v>286</v>
+      </c>
+      <c r="G72" t="s">
+        <v>290</v>
+      </c>
+      <c r="H72" t="s">
+        <v>317</v>
+      </c>
+      <c r="I72" t="s">
+        <v>338</v>
+      </c>
+      <c r="J72" t="s">
+        <v>383</v>
+      </c>
+      <c r="K72" t="s">
+        <v>448</v>
+      </c>
+      <c r="L72" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId2"/>
     <hyperlink ref="E5" r:id="rId3"/>
     <hyperlink ref="E6" r:id="rId4"/>
     <hyperlink ref="E7" r:id="rId5"/>
@@ -4102,43 +4549,48 @@
     <hyperlink ref="E15" r:id="rId12"/>
     <hyperlink ref="E16" r:id="rId13"/>
     <hyperlink ref="E17" r:id="rId14"/>
-    <hyperlink ref="E19" r:id="rId15"/>
-    <hyperlink ref="E20" r:id="rId16"/>
-    <hyperlink ref="E21" r:id="rId17"/>
-    <hyperlink ref="E22" r:id="rId18"/>
-    <hyperlink ref="E23" r:id="rId19"/>
-    <hyperlink ref="E25" r:id="rId20"/>
-    <hyperlink ref="E26" r:id="rId21"/>
-    <hyperlink ref="E27" r:id="rId22"/>
-    <hyperlink ref="E28" r:id="rId23"/>
-    <hyperlink ref="E29" r:id="rId24"/>
+    <hyperlink ref="E18" r:id="rId15"/>
+    <hyperlink ref="E19" r:id="rId16"/>
+    <hyperlink ref="E20" r:id="rId17"/>
+    <hyperlink ref="E21" r:id="rId18"/>
+    <hyperlink ref="E25" r:id="rId19"/>
+    <hyperlink ref="E26" r:id="rId20"/>
+    <hyperlink ref="E27" r:id="rId21"/>
+    <hyperlink ref="E28" r:id="rId22"/>
+    <hyperlink ref="E29" r:id="rId23"/>
+    <hyperlink ref="E31" r:id="rId24"/>
     <hyperlink ref="E32" r:id="rId25"/>
     <hyperlink ref="E33" r:id="rId26"/>
     <hyperlink ref="E34" r:id="rId27"/>
-    <hyperlink ref="E36" r:id="rId28"/>
-    <hyperlink ref="E37" r:id="rId29"/>
+    <hyperlink ref="E35" r:id="rId28"/>
+    <hyperlink ref="E36" r:id="rId29"/>
     <hyperlink ref="E39" r:id="rId30"/>
     <hyperlink ref="E40" r:id="rId31"/>
     <hyperlink ref="E41" r:id="rId32"/>
-    <hyperlink ref="E42" r:id="rId33"/>
-    <hyperlink ref="E43" r:id="rId34"/>
-    <hyperlink ref="E45" r:id="rId35"/>
-    <hyperlink ref="E46" r:id="rId36"/>
-    <hyperlink ref="E47" r:id="rId37"/>
+    <hyperlink ref="E43" r:id="rId33"/>
+    <hyperlink ref="E44" r:id="rId34"/>
+    <hyperlink ref="E46" r:id="rId35"/>
+    <hyperlink ref="E47" r:id="rId36"/>
+    <hyperlink ref="E48" r:id="rId37"/>
     <hyperlink ref="E49" r:id="rId38"/>
     <hyperlink ref="E50" r:id="rId39"/>
-    <hyperlink ref="E51" r:id="rId40"/>
-    <hyperlink ref="E52" r:id="rId41"/>
-    <hyperlink ref="E53" r:id="rId42"/>
-    <hyperlink ref="E54" r:id="rId43"/>
-    <hyperlink ref="E55" r:id="rId44"/>
-    <hyperlink ref="E57" r:id="rId45"/>
-    <hyperlink ref="E58" r:id="rId46"/>
-    <hyperlink ref="E59" r:id="rId47"/>
-    <hyperlink ref="E60" r:id="rId48"/>
-    <hyperlink ref="E61" r:id="rId49"/>
-    <hyperlink ref="E62" r:id="rId50"/>
-    <hyperlink ref="E63" r:id="rId51"/>
+    <hyperlink ref="E52" r:id="rId40"/>
+    <hyperlink ref="E53" r:id="rId41"/>
+    <hyperlink ref="E54" r:id="rId42"/>
+    <hyperlink ref="E56" r:id="rId43"/>
+    <hyperlink ref="E57" r:id="rId44"/>
+    <hyperlink ref="E58" r:id="rId45"/>
+    <hyperlink ref="E60" r:id="rId46"/>
+    <hyperlink ref="E61" r:id="rId47"/>
+    <hyperlink ref="E62" r:id="rId48"/>
+    <hyperlink ref="E63" r:id="rId49"/>
+    <hyperlink ref="E65" r:id="rId50"/>
+    <hyperlink ref="E66" r:id="rId51"/>
+    <hyperlink ref="E67" r:id="rId52"/>
+    <hyperlink ref="E68" r:id="rId53"/>
+    <hyperlink ref="E70" r:id="rId54"/>
+    <hyperlink ref="E71" r:id="rId55"/>
+    <hyperlink ref="E72" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>